<commit_message>
modificacoes dia 27-06-2025, configuracao dos envios dos formulario para o onedrive via api graph, ultimo horimetro configurado
</commit_message>
<xml_diff>
--- a/backend/planilhas/banco-de-dados-indicador.xlsx
+++ b/backend/planilhas/banco-de-dados-indicador.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -477,9 +477,61 @@
         <v>teste</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B4" t="str">
+        <v>27/06/2025, 13:31</v>
+      </c>
+      <c r="C4" t="str">
+        <v>WIVGH</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-06-27</v>
+      </c>
+      <c r="E4" t="str">
+        <v>25</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Mecânico</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Castanha/Cardã</v>
+      </c>
+      <c r="H4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>control system</v>
+      </c>
+      <c r="B5" t="str">
+        <v>27/06/2025, 13:34</v>
+      </c>
+      <c r="C5" t="str">
+        <v>FKB58</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-06-27</v>
+      </c>
+      <c r="E5" t="str">
+        <v>25</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Elétrico</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Anel Coletor</v>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>